<commit_message>
dã check dc Fab, pipe end, rundim 10.46_11.06
</commit_message>
<xml_diff>
--- a/Xp54-Fabrication & Listing.xlsx
+++ b/Xp54-Fabrication & Listing.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\05 Projects\2025\Endfire - WHTP2\03_Working\06_Published for QA checking\06_June\25.06.10_Xp53-54_Fabrication &amp; Listing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Desktop\thu nghien software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07EAD429-CD09-4174-999F-FCD15BE3A87F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F857C851-12E4-4FD7-8E48-2BD89355A8E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1BF4BFA9-A4F9-448D-B728-5188001683D6}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{1BF4BFA9-A4F9-448D-B728-5188001683D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Pipe Schedule" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3965" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3964" uniqueCount="138">
   <si>
     <t>EE_Cross Passage</t>
   </si>
@@ -947,11 +947,6 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1056,6 +1051,11 @@
       <numFmt numFmtId="164" formatCode="0.0"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1070,8 +1070,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{486292D6-46B7-4EDC-B885-535C17DDF0D0}" name="Table1" displayName="Table1" ref="A1:W93" totalsRowCount="1" totalsRowDxfId="23">
-  <autoFilter ref="A1:W92" xr:uid="{486292D6-46B7-4EDC-B885-535C17DDF0D0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{486292D6-46B7-4EDC-B885-535C17DDF0D0}" name="Table1" displayName="Table1" ref="A1:W93" totalsRowCount="1" totalsRowDxfId="51">
+  <autoFilter ref="A1:W92" xr:uid="{486292D6-46B7-4EDC-B885-535C17DDF0D0}">
+    <filterColumn colId="6">
+      <filters>
+        <filter val="65"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="10">
+      <filters>
+        <filter val="Fabrication"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="12">
+      <filters>
+        <filter val="BE"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="23">
     <tableColumn id="1" xr3:uid="{8E8B2183-CFCD-47E0-93AD-2AB954DC80C9}" name="EE_Cross Passage" totalsRowLabel="Total" totalsRowDxfId="22"/>
     <tableColumn id="2" xr3:uid="{97259683-D49E-443B-97B5-A168A904DD01}" name="EE_Location and Lanes" totalsRowDxfId="21"/>
@@ -1080,9 +1096,9 @@
     <tableColumn id="5" xr3:uid="{48A9103B-D927-4CF4-AF6C-6B8C33FEED3A}" name="EE_Stock Code" totalsRowDxfId="18"/>
     <tableColumn id="6" xr3:uid="{F2401C36-7CAE-4608-8B61-FF32E7B8E051}" name="EE_Item Description" totalsRowDxfId="17"/>
     <tableColumn id="7" xr3:uid="{7F4E6F01-BA6A-41D2-BC42-71C712E9E4C5}" name="Size" totalsRowDxfId="16"/>
-    <tableColumn id="8" xr3:uid="{FB7147C4-3B47-44A2-8F2C-8A061FBFE358}" name="Outside Diameter" dataDxfId="51" totalsRowDxfId="15"/>
-    <tableColumn id="9" xr3:uid="{5DED1B16-D4CE-4856-9171-FD7B34F4EA28}" name="Qty" totalsRowFunction="sum" dataDxfId="50" totalsRowDxfId="14"/>
-    <tableColumn id="10" xr3:uid="{19EFDECE-0ACB-4535-97DC-BE9A55F1BD75}" name="Length" dataDxfId="49" totalsRowDxfId="13"/>
+    <tableColumn id="8" xr3:uid="{FB7147C4-3B47-44A2-8F2C-8A061FBFE358}" name="Outside Diameter" dataDxfId="50" totalsRowDxfId="15"/>
+    <tableColumn id="9" xr3:uid="{5DED1B16-D4CE-4856-9171-FD7B34F4EA28}" name="Qty" totalsRowFunction="sum" dataDxfId="49" totalsRowDxfId="14"/>
+    <tableColumn id="10" xr3:uid="{19EFDECE-0ACB-4535-97DC-BE9A55F1BD75}" name="Length" dataDxfId="48" totalsRowDxfId="13"/>
     <tableColumn id="11" xr3:uid="{F1AD1177-A79C-4ED8-B27E-E114011BCDD8}" name="EE_FAB Pipe" totalsRowDxfId="12"/>
     <tableColumn id="12" xr3:uid="{F1BFCFBB-8AA2-49E3-A665-D085ADE045DA}" name="EE_PIPE END-1" totalsRowDxfId="11"/>
     <tableColumn id="13" xr3:uid="{FE9F6F41-1550-4848-AA21-DFCB2B3AD521}" name="EE_PIPE END-2" totalsRowDxfId="10"/>
@@ -1095,7 +1111,7 @@
     <tableColumn id="20" xr3:uid="{EDF669FD-7BE8-4749-959A-A3A6B2FA4EC3}" name="EE_Pipe Treatment" totalsRowDxfId="3"/>
     <tableColumn id="21" xr3:uid="{0A2495F1-87B3-47F0-BDF1-8E781B0E791B}" name="Family" totalsRowDxfId="2"/>
     <tableColumn id="22" xr3:uid="{311AA553-C69E-41E9-A087-259E88225C23}" name="Type" totalsRowDxfId="1"/>
-    <tableColumn id="23" xr3:uid="{C75BC3D9-4EFB-4CA2-BBCE-E308803D26B2}" name="ID" dataDxfId="48" totalsRowDxfId="0"/>
+    <tableColumn id="23" xr3:uid="{C75BC3D9-4EFB-4CA2-BBCE-E308803D26B2}" name="ID" dataDxfId="47" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1112,9 +1128,9 @@
     <tableColumn id="5" xr3:uid="{B001DCA7-BB3F-4C48-AF7F-079C147453E7}" name="EE_Stock Code"/>
     <tableColumn id="6" xr3:uid="{7FD96EB3-D7D8-4044-82A5-C913D192554C}" name="EE_Item Description"/>
     <tableColumn id="7" xr3:uid="{B93EBD4D-B308-4D41-AE3F-EBD87BA2814C}" name="Size"/>
-    <tableColumn id="8" xr3:uid="{1CBC1884-4E75-495E-9078-F5AAFE8DB68B}" name="Outside Diameter" dataDxfId="47" totalsRowDxfId="46"/>
-    <tableColumn id="9" xr3:uid="{D0DA34E5-395D-48B3-ADC8-7B8D08BBF812}" name="Qty" dataDxfId="45" totalsRowDxfId="44"/>
-    <tableColumn id="10" xr3:uid="{4E61F602-5E38-4165-AF1E-386FE3F25CA0}" name="Length" dataDxfId="43" totalsRowDxfId="42"/>
+    <tableColumn id="8" xr3:uid="{1CBC1884-4E75-495E-9078-F5AAFE8DB68B}" name="Outside Diameter" dataDxfId="46" totalsRowDxfId="45"/>
+    <tableColumn id="9" xr3:uid="{D0DA34E5-395D-48B3-ADC8-7B8D08BBF812}" name="Qty" dataDxfId="44" totalsRowDxfId="43"/>
+    <tableColumn id="10" xr3:uid="{4E61F602-5E38-4165-AF1E-386FE3F25CA0}" name="Length" dataDxfId="42" totalsRowDxfId="41"/>
     <tableColumn id="11" xr3:uid="{1912A30C-F4C1-4643-A1D3-E7C43E0BA728}" name="EE_FAB Pipe"/>
     <tableColumn id="12" xr3:uid="{74369ACD-B58E-4076-8068-8C2C485819D4}" name="EE_PIPE END-1"/>
     <tableColumn id="13" xr3:uid="{E75F0F0B-654F-4E90-8270-CE94886A115B}" name="EE_PIPE END-2"/>
@@ -1127,7 +1143,7 @@
     <tableColumn id="20" xr3:uid="{46EF927A-F887-4FB9-B1D7-B0283E488856}" name="EE_Pipe Treatment"/>
     <tableColumn id="21" xr3:uid="{93202F73-C8DE-459F-BA9E-32E9A65C4B4B}" name="Family"/>
     <tableColumn id="22" xr3:uid="{3F6D1BB0-25AC-4FA5-8B61-2BEEC4DFC3F5}" name="Type"/>
-    <tableColumn id="23" xr3:uid="{7E7D52DF-92F3-489A-9E62-14B6BBA2A257}" name="ID" totalsRowFunction="sum" dataDxfId="41" totalsRowDxfId="40"/>
+    <tableColumn id="23" xr3:uid="{7E7D52DF-92F3-489A-9E62-14B6BBA2A257}" name="ID" totalsRowFunction="sum" dataDxfId="40" totalsRowDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1144,9 +1160,9 @@
     <tableColumn id="5" xr3:uid="{03845035-80F4-4EA1-B192-2DC80C930925}" name="EE_Stock Code"/>
     <tableColumn id="6" xr3:uid="{BFC3452D-E9BC-436F-82D0-557B79C87BA4}" name="EE_Item Description"/>
     <tableColumn id="7" xr3:uid="{6B2C00F5-1F5A-49C0-B172-B57606B4018B}" name="Size"/>
-    <tableColumn id="8" xr3:uid="{911D545D-824C-410E-80E4-3B4FF82C2808}" name="Outside Diameter" dataDxfId="39" totalsRowDxfId="38"/>
-    <tableColumn id="9" xr3:uid="{89E68F50-6BEB-4C7E-AF6B-CC6F5D304384}" name="Qty" dataDxfId="37" totalsRowDxfId="36"/>
-    <tableColumn id="10" xr3:uid="{6709C980-DAC0-4593-BBCE-93FE1484AD5F}" name="Length" dataDxfId="35" totalsRowDxfId="34"/>
+    <tableColumn id="8" xr3:uid="{911D545D-824C-410E-80E4-3B4FF82C2808}" name="Outside Diameter" dataDxfId="38" totalsRowDxfId="37"/>
+    <tableColumn id="9" xr3:uid="{89E68F50-6BEB-4C7E-AF6B-CC6F5D304384}" name="Qty" dataDxfId="36" totalsRowDxfId="35"/>
+    <tableColumn id="10" xr3:uid="{6709C980-DAC0-4593-BBCE-93FE1484AD5F}" name="Length" dataDxfId="34" totalsRowDxfId="33"/>
     <tableColumn id="11" xr3:uid="{8A99CCA1-F897-4EFC-AD4C-2C9E381C7F00}" name="EE_FAB Pipe"/>
     <tableColumn id="12" xr3:uid="{9148E584-9EB0-4E9C-9917-3936990EEE39}" name="EE_PIPE END-1"/>
     <tableColumn id="13" xr3:uid="{580C8E8B-6C54-4BF6-ACD3-3F30954BE0F8}" name="EE_PIPE END-2"/>
@@ -1159,7 +1175,7 @@
     <tableColumn id="20" xr3:uid="{98261D20-7F4B-41A8-9D57-446FDFB0C366}" name="EE_Pipe Treatment"/>
     <tableColumn id="21" xr3:uid="{8829A659-1321-42CD-9CCB-CF7CC92DCEE4}" name="Family"/>
     <tableColumn id="22" xr3:uid="{7CB0F522-5FD8-4696-8049-39748C683E6E}" name="Type"/>
-    <tableColumn id="23" xr3:uid="{3B0EFBA6-DA36-4BB4-96B4-0EAC6C2EDF39}" name="ID" totalsRowFunction="sum" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="23" xr3:uid="{3B0EFBA6-DA36-4BB4-96B4-0EAC6C2EDF39}" name="ID" totalsRowFunction="sum" dataDxfId="32" totalsRowDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1179,9 +1195,9 @@
     <tableColumn id="5" xr3:uid="{1DAD6655-A28F-4894-ADD5-5DF3B46243E9}" name="EE_Stock Code"/>
     <tableColumn id="6" xr3:uid="{ECBAEC9D-D4C6-4864-A53C-2BA051A3EA02}" name="EE_Item Description"/>
     <tableColumn id="7" xr3:uid="{A707D78B-12DE-4C9F-934D-CC58E0D788ED}" name="Size"/>
-    <tableColumn id="8" xr3:uid="{DCAE458C-1AA6-4E44-9FFF-DCF66677FA54}" name="Outside Diameter" dataDxfId="31" totalsRowDxfId="30"/>
-    <tableColumn id="9" xr3:uid="{56CE60F4-A67F-4D96-8B06-1320C3D5C7B5}" name="Qty" dataDxfId="29" totalsRowDxfId="28"/>
-    <tableColumn id="10" xr3:uid="{B4BCE777-5951-4918-8F4D-B9B768482860}" name="Length" dataDxfId="27" totalsRowDxfId="26"/>
+    <tableColumn id="8" xr3:uid="{DCAE458C-1AA6-4E44-9FFF-DCF66677FA54}" name="Outside Diameter" dataDxfId="30" totalsRowDxfId="29"/>
+    <tableColumn id="9" xr3:uid="{56CE60F4-A67F-4D96-8B06-1320C3D5C7B5}" name="Qty" dataDxfId="28" totalsRowDxfId="27"/>
+    <tableColumn id="10" xr3:uid="{B4BCE777-5951-4918-8F4D-B9B768482860}" name="Length" dataDxfId="26" totalsRowDxfId="25"/>
     <tableColumn id="11" xr3:uid="{B53EC2ED-DDDB-4DBA-A176-6D1CBE8CB15C}" name="EE_FAB Pipe"/>
     <tableColumn id="12" xr3:uid="{98554396-A529-4238-A15C-850607A12D98}" name="EE_PIPE END-1"/>
     <tableColumn id="13" xr3:uid="{BE65BD6E-E33E-4579-977E-40D27B5906B3}" name="EE_PIPE END-2"/>
@@ -1194,7 +1210,7 @@
     <tableColumn id="20" xr3:uid="{354CD83F-8889-4378-8726-6535213AB664}" name="EE_Pipe Treatment"/>
     <tableColumn id="21" xr3:uid="{F820DB37-C0D4-44F9-B3AD-256EA475FA67}" name="Family"/>
     <tableColumn id="22" xr3:uid="{336D9F66-62BA-46E7-9163-905DAE22FB39}" name="Type"/>
-    <tableColumn id="23" xr3:uid="{DD9413AD-376E-41EB-89BC-CA048A8FEDAC}" name="ID" totalsRowFunction="sum" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="23" xr3:uid="{DD9413AD-376E-41EB-89BC-CA048A8FEDAC}" name="ID" totalsRowFunction="sum" dataDxfId="24" totalsRowDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1519,8 +1535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AF87CCC-1D52-42EF-B2E8-F518DD8AEB0B}">
   <dimension ref="A1:W93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J56"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N95" sqref="N95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1620,7 +1636,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -1673,7 +1689,7 @@
         <v>3658846</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -1720,7 +1736,7 @@
         <v>3658853</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -1767,7 +1783,7 @@
         <v>3658855</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -1814,7 +1830,7 @@
         <v>3658858</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1861,7 +1877,7 @@
         <v>3658861</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -1914,7 +1930,7 @@
         <v>3658881</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -1961,7 +1977,7 @@
         <v>3658883</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -2008,7 +2024,7 @@
         <v>3658899</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -2055,7 +2071,7 @@
         <v>3658907</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -2108,7 +2124,7 @@
         <v>3658924</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -2155,7 +2171,7 @@
         <v>3658926</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -2202,7 +2218,7 @@
         <v>3658932</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -2249,7 +2265,7 @@
         <v>3658937</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -2296,7 +2312,7 @@
         <v>3658940</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -2349,7 +2365,7 @@
         <v>3658959</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -2396,7 +2412,7 @@
         <v>3658961</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -2443,7 +2459,7 @@
         <v>3658977</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -2490,7 +2506,7 @@
         <v>3665401</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -2537,7 +2553,7 @@
         <v>3665404</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -2584,7 +2600,7 @@
         <v>3907537</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -2631,7 +2647,7 @@
         <v>3907554</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -2678,7 +2694,7 @@
         <v>3907580</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -2725,7 +2741,7 @@
         <v>3907586</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -2772,7 +2788,7 @@
         <v>3907614</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -2825,7 +2841,7 @@
         <v>3907650</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -2872,7 +2888,7 @@
         <v>3908004</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>23</v>
       </c>
@@ -2919,7 +2935,7 @@
         <v>3908190</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>23</v>
       </c>
@@ -2966,7 +2982,7 @@
         <v>3908251</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>23</v>
       </c>
@@ -3019,7 +3035,7 @@
         <v>4428450</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>23</v>
       </c>
@@ -3072,7 +3088,7 @@
         <v>4428460</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>23</v>
       </c>
@@ -3125,7 +3141,7 @@
         <v>4428489</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>23</v>
       </c>
@@ -3172,7 +3188,7 @@
         <v>4428491</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>23</v>
       </c>
@@ -3219,7 +3235,7 @@
         <v>4428496</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>23</v>
       </c>
@@ -3266,7 +3282,7 @@
         <v>4428500</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>23</v>
       </c>
@@ -3319,7 +3335,7 @@
         <v>4428518</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>23</v>
       </c>
@@ -3366,7 +3382,7 @@
         <v>4428520</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>23</v>
       </c>
@@ -3413,7 +3429,7 @@
         <v>4428531</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>23</v>
       </c>
@@ -3472,7 +3488,7 @@
         <v>4428637</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>23</v>
       </c>
@@ -3507,7 +3523,7 @@
         <v>29</v>
       </c>
       <c r="M40" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="T40" t="s">
         <v>32</v>
@@ -3554,10 +3570,7 @@
         <v>29</v>
       </c>
       <c r="M41" t="s">
-        <v>30</v>
-      </c>
-      <c r="N41">
-        <v>1107</v>
+        <v>29</v>
       </c>
       <c r="O41" t="s">
         <v>31</v>
@@ -3572,7 +3585,7 @@
         <v>4428696</v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>23</v>
       </c>
@@ -3619,7 +3632,7 @@
         <v>4428709</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>23</v>
       </c>
@@ -3666,7 +3679,7 @@
         <v>4428948</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>23</v>
       </c>
@@ -3713,7 +3726,7 @@
         <v>4428954</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>23</v>
       </c>
@@ -3760,7 +3773,7 @@
         <v>4428960</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>23</v>
       </c>
@@ -3807,7 +3820,7 @@
         <v>4429006</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>23</v>
       </c>
@@ -3854,7 +3867,7 @@
         <v>8177018</v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>23</v>
       </c>
@@ -3901,7 +3914,7 @@
         <v>8179306</v>
       </c>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>23</v>
       </c>
@@ -3960,7 +3973,7 @@
         <v>8179384</v>
       </c>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>23</v>
       </c>
@@ -4042,14 +4055,11 @@
         <v>29</v>
       </c>
       <c r="M51" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N51">
         <v>1108</v>
       </c>
-      <c r="O51" t="s">
-        <v>31</v>
-      </c>
       <c r="T51" t="s">
         <v>32</v>
       </c>
@@ -4060,7 +4070,7 @@
         <v>8179402</v>
       </c>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>23</v>
       </c>
@@ -4107,7 +4117,7 @@
         <v>8179408</v>
       </c>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>23</v>
       </c>
@@ -4154,7 +4164,7 @@
         <v>8179415</v>
       </c>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>23</v>
       </c>
@@ -4201,7 +4211,7 @@
         <v>8179420</v>
       </c>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>23</v>
       </c>
@@ -4248,7 +4258,7 @@
         <v>8179424</v>
       </c>
     </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>23</v>
       </c>
@@ -4307,7 +4317,7 @@
         <v>8179461</v>
       </c>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>23</v>
       </c>
@@ -4342,7 +4352,7 @@
         <v>29</v>
       </c>
       <c r="M57" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="T57" t="s">
         <v>32</v>
@@ -4389,7 +4399,7 @@
         <v>29</v>
       </c>
       <c r="M58" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N58">
         <v>1110</v>
@@ -4407,7 +4417,7 @@
         <v>8179479</v>
       </c>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>23</v>
       </c>
@@ -4454,7 +4464,7 @@
         <v>8179485</v>
       </c>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>23</v>
       </c>
@@ -4501,7 +4511,7 @@
         <v>8179501</v>
       </c>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>23</v>
       </c>
@@ -4548,7 +4558,7 @@
         <v>8180918</v>
       </c>
     </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>23</v>
       </c>
@@ -4595,7 +4605,7 @@
         <v>8180968</v>
       </c>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>23</v>
       </c>
@@ -4642,7 +4652,7 @@
         <v>8181275</v>
       </c>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>23</v>
       </c>
@@ -4689,7 +4699,7 @@
         <v>8181376</v>
       </c>
     </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>23</v>
       </c>
@@ -4736,7 +4746,7 @@
         <v>9164129</v>
       </c>
     </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>23</v>
       </c>
@@ -4783,7 +4793,7 @@
         <v>9164265</v>
       </c>
     </row>
-    <row r="67" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>23</v>
       </c>
@@ -4830,7 +4840,7 @@
         <v>9164297</v>
       </c>
     </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>23</v>
       </c>
@@ -4877,7 +4887,7 @@
         <v>9166387</v>
       </c>
     </row>
-    <row r="69" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>23</v>
       </c>
@@ -4924,7 +4934,7 @@
         <v>9166403</v>
       </c>
     </row>
-    <row r="70" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>23</v>
       </c>
@@ -4971,7 +4981,7 @@
         <v>9168798</v>
       </c>
     </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>23</v>
       </c>
@@ -5018,7 +5028,7 @@
         <v>9235594</v>
       </c>
     </row>
-    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>23</v>
       </c>
@@ -5065,7 +5075,7 @@
         <v>9235642</v>
       </c>
     </row>
-    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>23</v>
       </c>
@@ -5112,7 +5122,7 @@
         <v>9235667</v>
       </c>
     </row>
-    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>23</v>
       </c>
@@ -5159,7 +5169,7 @@
         <v>9235671</v>
       </c>
     </row>
-    <row r="75" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>23</v>
       </c>
@@ -5206,7 +5216,7 @@
         <v>12364294</v>
       </c>
     </row>
-    <row r="76" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>23</v>
       </c>
@@ -5253,7 +5263,7 @@
         <v>12364485</v>
       </c>
     </row>
-    <row r="77" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>23</v>
       </c>
@@ -5300,7 +5310,7 @@
         <v>12394731</v>
       </c>
     </row>
-    <row r="78" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>23</v>
       </c>
@@ -5347,7 +5357,7 @@
         <v>12394733</v>
       </c>
     </row>
-    <row r="79" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>23</v>
       </c>
@@ -5394,7 +5404,7 @@
         <v>12394735</v>
       </c>
     </row>
-    <row r="80" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>23</v>
       </c>
@@ -5441,7 +5451,7 @@
         <v>12574796</v>
       </c>
     </row>
-    <row r="81" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>23</v>
       </c>
@@ -5488,7 +5498,7 @@
         <v>12657003</v>
       </c>
     </row>
-    <row r="82" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>23</v>
       </c>
@@ -5535,7 +5545,7 @@
         <v>12657025</v>
       </c>
     </row>
-    <row r="83" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>23</v>
       </c>
@@ -5582,7 +5592,7 @@
         <v>12813851</v>
       </c>
     </row>
-    <row r="84" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>23</v>
       </c>
@@ -5629,7 +5639,7 @@
         <v>12827126</v>
       </c>
     </row>
-    <row r="85" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>23</v>
       </c>
@@ -5676,7 +5686,7 @@
         <v>14175157</v>
       </c>
     </row>
-    <row r="86" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>23</v>
       </c>
@@ -5723,7 +5733,7 @@
         <v>14175283</v>
       </c>
     </row>
-    <row r="87" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>23</v>
       </c>
@@ -5770,7 +5780,7 @@
         <v>14175345</v>
       </c>
     </row>
-    <row r="88" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>23</v>
       </c>
@@ -5817,7 +5827,7 @@
         <v>14175367</v>
       </c>
     </row>
-    <row r="89" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>23</v>
       </c>
@@ -5864,7 +5874,7 @@
         <v>14175621</v>
       </c>
     </row>
-    <row r="90" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>23</v>
       </c>
@@ -5911,7 +5921,7 @@
         <v>14175633</v>
       </c>
     </row>
-    <row r="91" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>23</v>
       </c>
@@ -5958,7 +5968,7 @@
         <v>14175751</v>
       </c>
     </row>
-    <row r="92" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>23</v>
       </c>
@@ -6018,7 +6028,7 @@
       <c r="H93" s="5"/>
       <c r="I93" s="6">
         <f>SUBTOTAL(109,Table1[Qty])</f>
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="J93" s="5"/>
       <c r="K93" s="4"/>
@@ -13882,8 +13892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBEF1045-B583-4A28-B51F-4FA9F6D3DCDE}">
   <dimension ref="A1:W107"/>
   <sheetViews>
-    <sheetView topLeftCell="A68" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C113" sqref="C113"/>
+    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13904,8 +13914,8 @@
     <col min="15" max="15" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.7109375" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="11.140625" hidden="1" customWidth="1"/>
     <col min="20" max="20" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="34.5703125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="27.42578125" bestFit="1" customWidth="1"/>

</xml_diff>